<commit_message>
add change pw form, validate only admin can CUD schedule
</commit_message>
<xml_diff>
--- a/Activity_adalah_aktivitas.xlsx
+++ b/Activity_adalah_aktivitas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN_10\Documents\computerScience\ITDiv\Final\rec-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD0FB1F5-3441-42A3-91E3-1F05D1D56D2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D398763-47BF-4E40-8651-DBE0C7A1320B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3B294C3-DDED-4FFB-B8E3-505CE2EFF63E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Target (controller stuff/backend)</t>
   </si>
@@ -119,9 +119,6 @@
     <t>insert skedul dibuatin button, yg buka modal (popup)</t>
   </si>
   <si>
-    <t>validasi admin doang yg bisa add skedul</t>
-  </si>
-  <si>
     <t>mengecek cara pisah datenya sama timenya, karena di tampilannya dia bakal beda</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>waduh</t>
+  </si>
+  <si>
+    <t>validasi admin doang yg bisa add/delete/update skedul</t>
   </si>
 </sst>
 </file>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F319736C-32FD-41A0-A96F-32FDC20D3086}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,103 +647,109 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add token to reset password
</commit_message>
<xml_diff>
--- a/Activity_adalah_aktivitas.xlsx
+++ b/Activity_adalah_aktivitas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN_10\Documents\computerScience\ITDiv\Final\rec-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D398763-47BF-4E40-8651-DBE0C7A1320B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019FED2-F66B-4FD7-BCA9-D1209B391C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3B294C3-DDED-4FFB-B8E3-505CE2EFF63E}"/>
   </bookViews>
@@ -512,13 +512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F319736C-32FD-41A0-A96F-32FDC20D3086}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>